<commit_message>
changes to add browser details
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>UserName</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>abcd@xyz.com</t>
+  </si>
+  <si>
+    <t>Completed</t>
   </si>
 </sst>
 </file>
@@ -361,7 +364,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
@@ -388,6 +391,9 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>